<commit_message>
Update Pixel to position encoding transformation.xlsx
</commit_message>
<xml_diff>
--- a/weibull/issues/Pixel to position encoding transformation.xlsx
+++ b/weibull/issues/Pixel to position encoding transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miked\Documents\GitHub\nmcuration\weibull\issues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F0B4874-B30E-401D-8607-DA70DC59C2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D760DD11-60F9-41E4-ACD5-9D0F13B4384E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{579AD940-E595-42B8-9D8F-3345B66182C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{579AD940-E595-42B8-9D8F-3345B66182C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>